<commit_message>
Visualisation - mise en forme légende et graphiques
</commit_message>
<xml_diff>
--- a/img/plot_legends.xlsx
+++ b/img/plot_legends.xlsx
@@ -811,10 +811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R44"/>
+  <dimension ref="B2:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,11 +830,11 @@
     <col min="9" max="9" width="8" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="9"/>
     <col min="11" max="11" width="3.5703125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.5703125" style="9" customWidth="1"/>
     <col min="14" max="14" width="21.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.5703125" style="9" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.5703125" style="9" customWidth="1"/>
     <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.5703125" style="9" customWidth="1"/>
@@ -842,8 +842,8 @@
     <col min="21" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>29</v>
       </c>
@@ -851,7 +851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" s="13" t="s">
         <v>0</v>
@@ -880,16 +880,12 @@
       <c r="P4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
     </row>
-    <row r="6" spans="2:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="13" t="s">
         <v>8</v>
@@ -906,53 +902,57 @@
       <c r="I6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="13" t="s">
+      <c r="O6" s="5"/>
+      <c r="P6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
     </row>
-    <row r="8" spans="2:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K8" s="21"/>
+    <row r="8" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="6"/>
       <c r="L8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="21"/>
+      <c r="P8" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="2:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="2:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
     </row>
-    <row r="14" spans="2:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="2:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>

</xml_diff>

<commit_message>
Visualisation - Légende prod grandes filières
</commit_message>
<xml_diff>
--- a/img/plot_legends.xlsx
+++ b/img/plot_legends.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Energie</t>
   </si>
@@ -106,6 +106,39 @@
   </si>
   <si>
     <t>Secteurs d'activité</t>
+  </si>
+  <si>
+    <t>Hydraulique</t>
+  </si>
+  <si>
+    <t>Eolien</t>
+  </si>
+  <si>
+    <t>Solaire Photovoltaïque</t>
+  </si>
+  <si>
+    <t>Bioénergies</t>
+  </si>
+  <si>
+    <t>Centrales Thermiques</t>
+  </si>
+  <si>
+    <t>Cogénération</t>
+  </si>
+  <si>
+    <t>Incinération des déchets industriels</t>
+  </si>
+  <si>
+    <t>Thermique fossile autres</t>
+  </si>
+  <si>
+    <t>Solaire Thermique</t>
+  </si>
+  <si>
+    <t>Récupération de chaleur</t>
+  </si>
+  <si>
+    <t>Grandes filières</t>
   </si>
 </sst>
 </file>
@@ -136,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +239,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCFF4C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA89561"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE50909"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -248,6 +293,8 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,16 +303,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE50909"/>
+      <color rgb="FF848484"/>
+      <color rgb="FFA89561"/>
+      <color rgb="FF33AFFF"/>
+      <color rgb="FF2E2EFE"/>
       <color rgb="FFFCFF4C"/>
       <color rgb="FF999999"/>
-      <color rgb="FF848484"/>
       <color rgb="FFC733FF"/>
       <color rgb="FFFF3390"/>
       <color rgb="FF33FF9C"/>
-      <color rgb="FF2E2EFE"/>
-      <color rgb="FF33AFFF"/>
-      <color rgb="FFFFBE33"/>
-      <color rgb="FFE97401"/>
     </mruColors>
   </colors>
   <extLst>
@@ -814,7 +861,7 @@
   <dimension ref="B2:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,15 +1000,71 @@
       <c r="C15" s="13"/>
     </row>
     <row r="16" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
     </row>
-    <row r="18" spans="2:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="4"/>
+      <c r="L21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="5"/>
+      <c r="N21" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" s="8"/>
+      <c r="P21" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="3"/>
+      <c r="L23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="23"/>
+      <c r="N23" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="24"/>
+      <c r="P23" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="2"/>
+      <c r="L25" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" s="6"/>
+      <c r="N25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O25" s="7"/>
+      <c r="P25" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="1"/>
+      <c r="L27" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="13"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Prod - Modification des filières
</commit_message>
<xml_diff>
--- a/img/plot_legends.xlsx
+++ b/img/plot_legends.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Energie</t>
   </si>
@@ -139,6 +139,45 @@
   </si>
   <si>
     <t>Grandes filières</t>
+  </si>
+  <si>
+    <t>ENR</t>
+  </si>
+  <si>
+    <t>Incinération</t>
+  </si>
+  <si>
+    <t>Grandes filières (ancienne version plus utilisée</t>
+  </si>
+  <si>
+    <t>id_detail_filiere_cigale</t>
+  </si>
+  <si>
+    <t>detail_filiere_cigale</t>
+  </si>
+  <si>
+    <t>Biogaz</t>
+  </si>
+  <si>
+    <t>Biomasse</t>
+  </si>
+  <si>
+    <t>Grande hydraulique</t>
+  </si>
+  <si>
+    <t>Incinération des ordures ménagères</t>
+  </si>
+  <si>
+    <t>Petite hydraulique</t>
+  </si>
+  <si>
+    <t>Pompes à chaleur</t>
+  </si>
+  <si>
+    <t>Solaire photovoltaïque</t>
+  </si>
+  <si>
+    <t>Solaire thermique</t>
   </si>
 </sst>
 </file>
@@ -858,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P44"/>
+  <dimension ref="B2:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +923,7 @@
     <col min="16" max="16" width="21.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.5703125" style="9" customWidth="1"/>
     <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.5703125" style="9" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" style="9" customWidth="1"/>
     <col min="20" max="20" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="11.42578125" style="9"/>
   </cols>
@@ -1011,79 +1050,198 @@
       </c>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K21" s="4"/>
+      <c r="K21" s="5"/>
       <c r="L21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P21" s="13"/>
+    </row>
+    <row r="22" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="23"/>
+      <c r="L23" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="6"/>
+      <c r="L25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25" s="13"/>
+    </row>
+    <row r="26" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="24"/>
+      <c r="L27" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="4"/>
+      <c r="L30" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M21" s="5"/>
-      <c r="N21" s="13" t="s">
+      <c r="M30" s="5"/>
+      <c r="N30" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="8"/>
-      <c r="P21" s="13" t="s">
+      <c r="O30" s="8"/>
+      <c r="P30" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="3"/>
-      <c r="L23" s="13" t="s">
+    <row r="31" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="3"/>
+      <c r="L32" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="23"/>
-      <c r="N23" s="13" t="s">
+      <c r="M32" s="23"/>
+      <c r="N32" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="24"/>
-      <c r="P23" s="13" t="s">
+      <c r="O32" s="24"/>
+      <c r="P32" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K25" s="2"/>
-      <c r="L25" s="13" t="s">
+    <row r="33" spans="2:23" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+      <c r="L34" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="6"/>
-      <c r="N25" s="13" t="s">
+      <c r="M34" s="6"/>
+      <c r="N34" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="7"/>
-      <c r="P25" s="13" t="s">
+      <c r="O34" s="7"/>
+      <c r="P34" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="1"/>
-      <c r="L27" s="13" t="s">
+    <row r="35" spans="2:23" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="1"/>
+      <c r="L36" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="13"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="13"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B40" s="13"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="V40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="W40" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U41" s="5"/>
+      <c r="V41" s="9">
+        <v>5</v>
+      </c>
+      <c r="W41" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B42" s="13"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="U42" s="3"/>
+      <c r="V42" s="9">
+        <v>9</v>
+      </c>
+      <c r="W42" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U43" s="4"/>
+      <c r="V43" s="9">
+        <v>6</v>
+      </c>
+      <c r="W43" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B44" s="13"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="9">
+        <v>12</v>
+      </c>
+      <c r="W44" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U45" s="1"/>
+      <c r="V45" s="9">
+        <v>13</v>
+      </c>
+      <c r="W45" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B46" s="13"/>
+      <c r="U46" s="23"/>
+      <c r="V46" s="9">
+        <v>1</v>
+      </c>
+      <c r="W46" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U47" s="6"/>
+      <c r="V47" s="9">
+        <v>2</v>
+      </c>
+      <c r="W47" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B48" s="13"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="9">
+        <v>10</v>
+      </c>
+      <c r="W48" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U49" s="8"/>
+      <c r="V49" s="9">
+        <v>8</v>
+      </c>
+      <c r="W49" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B50" s="13"/>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B52" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MAJ 2019 Passage en classes PCAET, changement logo, ...
</commit_message>
<xml_diff>
--- a/img/plot_legends.xlsx
+++ b/img/plot_legends.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>Energie</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Solaire thermique</t>
+  </si>
+  <si>
+    <t>Secteurs PCAET</t>
+  </si>
+  <si>
+    <t>Déchets</t>
+  </si>
+  <si>
+    <t>Industrie</t>
   </si>
 </sst>
 </file>
@@ -208,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE50909"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF534629"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -334,6 +349,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,6 +359,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF534629"/>
+      <color rgb="FFFFD57D"/>
       <color rgb="FFE50909"/>
       <color rgb="FF848484"/>
       <color rgb="FFA89561"/>
@@ -350,8 +369,6 @@
       <color rgb="FFFCFF4C"/>
       <color rgb="FF999999"/>
       <color rgb="FFC733FF"/>
-      <color rgb="FFFF3390"/>
-      <color rgb="FF33FF9C"/>
     </mruColors>
   </colors>
   <extLst>
@@ -899,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="U49" sqref="U49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,9 +926,9 @@
     <col min="2" max="2" width="3.5703125" style="9" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="9" customWidth="1"/>
     <col min="6" max="6" width="3.5703125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="9" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" style="9" customWidth="1"/>
     <col min="9" max="9" width="8" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="9"/>
@@ -1024,21 +1041,70 @@
       <c r="C9" s="13"/>
     </row>
     <row r="10" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="22"/>
+    </row>
+    <row r="12" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="2:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="9"/>
+      <c r="O13" s="25"/>
+    </row>
+    <row r="14" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="19"/>
+      <c r="I14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="13"/>
+    </row>
+    <row r="15" spans="2:16" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="20"/>
+      <c r="C16" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>

</xml_diff>